<commit_message>
change latitude for station 44
</commit_message>
<xml_diff>
--- a/chimie/tests/PIRATA FR 25_chimie.xlsx
+++ b/chimie/tests/PIRATA FR 25_chimie.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-720" yWindow="-75" windowWidth="8865" windowHeight="5700" activeTab="4"/>
+    <workbookView xWindow="-720" yWindow="-75" windowWidth="8865" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="041_01" sheetId="4" r:id="rId1"/>
@@ -2650,7 +2650,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12397671693252373"/>
+          <c:x val="0.12397671693252375"/>
           <c:y val="7.4385552552199627E-2"/>
           <c:w val="0.77517854548624221"/>
           <c:h val="0.89521395646439761"/>
@@ -2754,11 +2754,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="145563648"/>
-        <c:axId val="145565952"/>
+        <c:axId val="103902208"/>
+        <c:axId val="103917056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145563648"/>
+        <c:axId val="103902208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2790,12 +2790,12 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145565952"/>
+        <c:crossAx val="103917056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145565952"/>
+        <c:axId val="103917056"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2828,7 +2828,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145563648"/>
+        <c:crossAx val="103902208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2838,7 +2838,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2857,9 +2857,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.13261013377045341"/>
-          <c:y val="7.7702302137606052E-2"/>
+          <c:y val="7.7702302137606094E-2"/>
           <c:w val="0.78042794836519069"/>
-          <c:h val="0.89189720687899188"/>
+          <c:h val="0.8918972068789921"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2960,11 +2960,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="178799744"/>
-        <c:axId val="178801664"/>
+        <c:axId val="104591360"/>
+        <c:axId val="104593280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178799744"/>
+        <c:axId val="104591360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,19 +2989,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.81219330855018712"/>
+              <c:x val="0.81219330855018734"/>
               <c:y val="7.3508050299682687E-2"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178801664"/>
+        <c:crossAx val="104593280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178801664"/>
+        <c:axId val="104593280"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3034,7 +3034,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178799744"/>
+        <c:crossAx val="104591360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3044,7 +3044,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3063,9 +3063,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.13261013377045341"/>
-          <c:y val="7.7702302137605997E-2"/>
+          <c:y val="7.7702302137606025E-2"/>
           <c:w val="0.78042794836519069"/>
-          <c:h val="0.89189720687899143"/>
+          <c:h val="0.89189720687899166"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3166,11 +3166,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="145594240"/>
-        <c:axId val="145600512"/>
+        <c:axId val="103937152"/>
+        <c:axId val="103939072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145594240"/>
+        <c:axId val="103937152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3195,19 +3195,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.81219330855018657"/>
+              <c:x val="0.8121933085501869"/>
               <c:y val="7.3508050299682687E-2"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145600512"/>
+        <c:crossAx val="103939072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145600512"/>
+        <c:axId val="103939072"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3240,7 +3240,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145594240"/>
+        <c:crossAx val="103937152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3250,7 +3250,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3268,7 +3268,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12397671693252373"/>
+          <c:x val="0.12397671693252375"/>
           <c:y val="7.4385552552199627E-2"/>
           <c:w val="0.77517854548624221"/>
           <c:h val="0.89521395646439761"/>
@@ -3372,11 +3372,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="145611776"/>
-        <c:axId val="154231936"/>
+        <c:axId val="104270080"/>
+        <c:axId val="104288640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145611776"/>
+        <c:axId val="104270080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3408,12 +3408,12 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154231936"/>
+        <c:crossAx val="104288640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154231936"/>
+        <c:axId val="104288640"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3446,7 +3446,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145611776"/>
+        <c:crossAx val="104270080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3456,7 +3456,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3475,9 +3475,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.13261013377045341"/>
-          <c:y val="7.7702302137605997E-2"/>
+          <c:y val="7.7702302137606025E-2"/>
           <c:w val="0.78042794836519069"/>
-          <c:h val="0.89189720687899143"/>
+          <c:h val="0.89189720687899166"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3578,11 +3578,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="154256128"/>
-        <c:axId val="154258048"/>
+        <c:axId val="104325120"/>
+        <c:axId val="104327040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154256128"/>
+        <c:axId val="104325120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3607,19 +3607,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.81219330855018657"/>
+              <c:x val="0.8121933085501869"/>
               <c:y val="7.3508050299682687E-2"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154258048"/>
+        <c:crossAx val="104327040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154258048"/>
+        <c:axId val="104327040"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3652,7 +3652,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154256128"/>
+        <c:crossAx val="104325120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3662,7 +3662,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3680,7 +3680,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12397671693252373"/>
+          <c:x val="0.12397671693252375"/>
           <c:y val="7.4385552552199627E-2"/>
           <c:w val="0.77517854548624221"/>
           <c:h val="0.89521395646439761"/>
@@ -3784,11 +3784,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="154662784"/>
-        <c:axId val="154542080"/>
+        <c:axId val="104420480"/>
+        <c:axId val="104422400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154662784"/>
+        <c:axId val="104420480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3820,12 +3820,12 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154542080"/>
+        <c:crossAx val="104422400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154542080"/>
+        <c:axId val="104422400"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3858,7 +3858,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154662784"/>
+        <c:crossAx val="104420480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3868,7 +3868,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3887,9 +3887,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.13261013377045341"/>
-          <c:y val="7.7702302137605997E-2"/>
+          <c:y val="7.7702302137606025E-2"/>
           <c:w val="0.78042794836519069"/>
-          <c:h val="0.89189720687899143"/>
+          <c:h val="0.89189720687899166"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3990,11 +3990,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="154553728"/>
-        <c:axId val="154572288"/>
+        <c:axId val="104454784"/>
+        <c:axId val="104469248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154553728"/>
+        <c:axId val="104454784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4019,19 +4019,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.81219330855018657"/>
+              <c:x val="0.8121933085501869"/>
               <c:y val="7.3508050299682687E-2"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154572288"/>
+        <c:crossAx val="104469248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154572288"/>
+        <c:axId val="104469248"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4064,7 +4064,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154553728"/>
+        <c:crossAx val="104454784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4074,7 +4074,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4092,7 +4092,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12397671693252375"/>
+          <c:x val="0.12397671693252378"/>
           <c:y val="7.4385552552199627E-2"/>
           <c:w val="0.77517854548624221"/>
           <c:h val="0.89521395646439761"/>
@@ -4196,11 +4196,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="154677632"/>
-        <c:axId val="154679552"/>
+        <c:axId val="104476032"/>
+        <c:axId val="104617472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154677632"/>
+        <c:axId val="104476032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4232,12 +4232,12 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154679552"/>
+        <c:crossAx val="104617472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154679552"/>
+        <c:axId val="104617472"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4270,7 +4270,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154677632"/>
+        <c:crossAx val="104476032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4280,7 +4280,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4299,9 +4299,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.13261013377045341"/>
-          <c:y val="7.7702302137606025E-2"/>
+          <c:y val="7.7702302137606052E-2"/>
           <c:w val="0.78042794836519069"/>
-          <c:h val="0.89189720687899166"/>
+          <c:h val="0.89189720687899188"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4402,11 +4402,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="154699648"/>
-        <c:axId val="154718208"/>
+        <c:axId val="104641664"/>
+        <c:axId val="104643584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154699648"/>
+        <c:axId val="104641664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4431,19 +4431,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.8121933085501869"/>
+              <c:x val="0.81219330855018712"/>
               <c:y val="7.3508050299682687E-2"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154718208"/>
+        <c:crossAx val="104643584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154718208"/>
+        <c:axId val="104643584"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4476,7 +4476,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154699648"/>
+        <c:crossAx val="104641664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4486,7 +4486,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4504,7 +4504,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12397671693252378"/>
+          <c:x val="0.12397671693252379"/>
           <c:y val="7.4385552552199627E-2"/>
           <c:w val="0.77517854548624221"/>
           <c:h val="0.89521395646439761"/>
@@ -4608,11 +4608,11 @@
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
         </c:dLbls>
-        <c:axId val="178769280"/>
-        <c:axId val="178787840"/>
+        <c:axId val="104536320"/>
+        <c:axId val="104550784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178769280"/>
+        <c:axId val="104536320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4644,12 +4644,12 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178787840"/>
+        <c:crossAx val="104550784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178787840"/>
+        <c:axId val="104550784"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4682,7 +4682,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178769280"/>
+        <c:crossAx val="104536320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4692,7 +4692,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5328,7 +5328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T34" sqref="T34:AC44"/>
     </sheetView>
   </sheetViews>
@@ -8346,7 +8346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P10" sqref="P10:R10"/>
     </sheetView>
   </sheetViews>
@@ -11127,7 +11127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView topLeftCell="H14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U34" sqref="U34:AC44"/>
     </sheetView>
   </sheetViews>
@@ -13928,8 +13928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34:AC44"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9:R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -14140,8 +14140,7 @@
         <v>32</v>
       </c>
       <c r="Q9" s="246">
-        <f>IF(ISBLANK(I9),"",IF(ISBLANK(J9),"",IF(J9&gt;60,"ERREUR !!",O11*(I9+(J9/60)))))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R9" s="247"/>
     </row>
@@ -16841,8 +16840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17053,8 +17052,7 @@
         <v>32</v>
       </c>
       <c r="Q9" s="246">
-        <f>IF(ISBLANK(I9),"",IF(ISBLANK(J9),"",IF(J9&gt;60,"ERREUR !!",O11*(I9+(J9/60)))))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R9" s="247"/>
     </row>

</xml_diff>